<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-ig-2@a7f12c0da64c729610ea9cc1fd369d98a048a7d7 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-SharedDataModelAliquot.xlsx
+++ b/StructureDefinition-SharedDataModelAliquot.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-08-20T21:48:07+00:00</t>
+    <t>2024-08-22T16:27:20+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -277,7 +277,7 @@
     <t>Can this Sample be requested for further analysis?</t>
   </si>
   <si>
-    <t>SharedDataModelAliquot.quantity</t>
+    <t>SharedDataModelAliquot.volume</t>
   </si>
   <si>
     <t xml:space="preserve">Quantity

</xml_diff>